<commit_message>
Testcases and Plots - iter 1.0
</commit_message>
<xml_diff>
--- a/Testcases_Part2.xlsx
+++ b/Testcases_Part2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Academics\Semester7\BTP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1060BB-45F4-4E48-AB92-11BA57D6B4BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F43C13-7F90-428F-A179-EEFB374705DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{82200626-AD99-4240-B52B-FF0FA02B1A32}"/>
   </bookViews>
@@ -149,7 +149,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,6 +198,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -235,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -246,6 +252,8 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,7 +571,7 @@
   <dimension ref="D2:S26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,7 +674,7 @@
       </c>
       <c r="O7" s="6">
         <f>IF(OR($N$7:$N$11)=0, 2, O8)</f>
-        <v>1.0000000000000009E-2</v>
+        <v>3.999999999999998E-2</v>
       </c>
       <c r="P7" s="6">
         <f>ABS(MIN(F7:J7)-L7)</f>
@@ -699,7 +707,7 @@
         <v>0.5</v>
       </c>
       <c r="H8" s="2">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="I8" s="2">
         <v>0.4</v>
@@ -709,7 +717,7 @@
       </c>
       <c r="K8" s="3">
         <f t="shared" ref="K8:K11" si="0">SUM(F8:J8)/5</f>
-        <v>0.57999999999999996</v>
+        <v>0.52</v>
       </c>
       <c r="L8" s="4">
         <v>0.35</v>
@@ -724,7 +732,7 @@
       </c>
       <c r="O8" s="6">
         <f>ABS($K$7-K8)/2</f>
-        <v>1.0000000000000009E-2</v>
+        <v>3.999999999999998E-2</v>
       </c>
       <c r="P8" s="6">
         <f t="shared" ref="P8:P11" si="2">ABS(MIN(F8:J8)-L8)</f>
@@ -732,7 +740,7 @@
       </c>
       <c r="Q8" s="7">
         <f t="shared" ref="Q8:Q11" si="3">(M8*N8/O8)^2</f>
-        <v>9999.9999999999836</v>
+        <v>625.00000000000068</v>
       </c>
       <c r="R8" s="7">
         <f t="shared" ref="R8:R11" si="4">((1-M8)*(1-N8)/P8)^2</f>
@@ -747,8 +755,8 @@
       <c r="E9" s="1">
         <v>3</v>
       </c>
-      <c r="F9" s="2">
-        <v>0.2</v>
+      <c r="F9" s="10">
+        <v>0.34</v>
       </c>
       <c r="G9" s="2">
         <v>0.5</v>
@@ -764,7 +772,7 @@
       </c>
       <c r="K9" s="3">
         <f t="shared" si="0"/>
-        <v>0.66</v>
+        <v>0.68799999999999994</v>
       </c>
       <c r="L9" s="4">
         <v>0.35</v>
@@ -779,11 +787,11 @@
       </c>
       <c r="O9" s="6">
         <f t="shared" ref="O9:O11" si="7">ABS($K$7-K9)/2</f>
-        <v>3.0000000000000027E-2</v>
+        <v>4.3999999999999984E-2</v>
       </c>
       <c r="P9" s="6">
         <f t="shared" si="2"/>
-        <v>0.14999999999999997</v>
+        <v>9.9999999999999534E-3</v>
       </c>
       <c r="Q9" s="7">
         <f t="shared" si="3"/>
@@ -791,7 +799,7 @@
       </c>
       <c r="R9" s="7">
         <f t="shared" si="4"/>
-        <v>44.444444444444457</v>
+        <v>10000.000000000095</v>
       </c>
       <c r="S9" s="7">
         <f t="shared" si="5"/>
@@ -925,15 +933,15 @@
     <row r="16" spans="4:19" x14ac:dyDescent="0.3">
       <c r="H16">
         <f>1/(MIN($O$7/2,$P$7))^2</f>
-        <v>39999.999999999927</v>
+        <v>2500.0000000000027</v>
       </c>
       <c r="I16">
         <f>SUM(Q7:Q11)</f>
-        <v>9999.9999999999836</v>
+        <v>625.00000000000068</v>
       </c>
       <c r="J16">
         <f>SUM(R7:R11)</f>
-        <v>44.444444444444457</v>
+        <v>10000.000000000095</v>
       </c>
       <c r="K16">
         <f>SUM(S7:S11)</f>
@@ -987,7 +995,7 @@
       </c>
       <c r="H23">
         <f t="shared" si="9"/>
-        <v>0.4285714285714286</v>
+        <v>1.5</v>
       </c>
       <c r="I23">
         <f t="shared" si="9"/>
@@ -999,9 +1007,9 @@
       </c>
     </row>
     <row r="24" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F24">
-        <f t="shared" si="9"/>
-        <v>4</v>
+      <c r="F24" s="11">
+        <f t="shared" si="9"/>
+        <v>1.9411764705882351</v>
       </c>
       <c r="G24">
         <f t="shared" si="9"/>
@@ -1073,8 +1081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E8C833E-65B9-41B5-89D0-A1D2541BD3C5}">
   <dimension ref="D6:U27"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1175,7 +1183,7 @@
       </c>
       <c r="O7" s="6">
         <f>IF(OR($N$7:$N$11)=0, 2, O8)</f>
-        <v>1.0000000000000009E-2</v>
+        <v>3.999999999999998E-2</v>
       </c>
       <c r="P7" s="6">
         <f>ABS(MIN(F7:J7)-L7)</f>
@@ -1212,7 +1220,7 @@
         <v>0.5</v>
       </c>
       <c r="H8" s="2">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="I8" s="2">
         <v>0.4</v>
@@ -1222,7 +1230,7 @@
       </c>
       <c r="K8" s="3">
         <f t="shared" ref="K8:K11" si="0">SUM(F8:J8)/5</f>
-        <v>0.57999999999999996</v>
+        <v>0.52</v>
       </c>
       <c r="L8" s="4">
         <v>0.35</v>
@@ -1237,7 +1245,7 @@
       </c>
       <c r="O8" s="6">
         <f>ABS($K$7-K8)/2</f>
-        <v>1.0000000000000009E-2</v>
+        <v>3.999999999999998E-2</v>
       </c>
       <c r="P8" s="6">
         <f t="shared" ref="P8:P11" si="2">ABS(MIN(F8:J8)-L8)</f>
@@ -1245,7 +1253,7 @@
       </c>
       <c r="Q8" s="7">
         <f t="shared" ref="Q8:Q11" si="3">(M8*N8/O8)^2</f>
-        <v>9999.9999999999836</v>
+        <v>625.00000000000068</v>
       </c>
       <c r="R8" s="7">
         <f t="shared" ref="R8:R11" si="4">((1-M8)*(1-N8)/P8)^2</f>
@@ -1264,8 +1272,8 @@
       <c r="E9" s="1">
         <v>3</v>
       </c>
-      <c r="F9" s="2">
-        <v>0.01</v>
+      <c r="F9" s="10">
+        <v>0.25</v>
       </c>
       <c r="G9" s="2">
         <v>0.5</v>
@@ -1281,7 +1289,7 @@
       </c>
       <c r="K9" s="3">
         <f t="shared" si="0"/>
-        <v>0.42199999999999999</v>
+        <v>0.47000000000000003</v>
       </c>
       <c r="L9" s="4">
         <v>0.35</v>
@@ -1296,11 +1304,11 @@
       </c>
       <c r="O9" s="6">
         <f t="shared" ref="O9:O11" si="8">ABS($K$7-K9)/2</f>
-        <v>8.8999999999999996E-2</v>
+        <v>6.4999999999999974E-2</v>
       </c>
       <c r="P9" s="6">
         <f t="shared" si="2"/>
-        <v>0.33999999999999997</v>
+        <v>9.9999999999999978E-2</v>
       </c>
       <c r="Q9" s="7">
         <f t="shared" si="3"/>
@@ -1312,7 +1320,7 @@
       </c>
       <c r="S9" s="7">
         <f t="shared" si="5"/>
-        <v>8.6505190311418705</v>
+        <v>100.00000000000003</v>
       </c>
       <c r="U9" t="b">
         <f t="shared" si="6"/>
@@ -1454,11 +1462,11 @@
     <row r="16" spans="4:21" x14ac:dyDescent="0.3">
       <c r="H16">
         <f>1/(MIN($O$7/2,$P$7))^2</f>
-        <v>39999.999999999927</v>
+        <v>2500.0000000000027</v>
       </c>
       <c r="I16">
         <f>SUM(Q7:Q11)</f>
-        <v>9999.9999999999836</v>
+        <v>625.00000000000068</v>
       </c>
       <c r="J16">
         <f>SUM(R7:R11)</f>
@@ -1466,7 +1474,7 @@
       </c>
       <c r="K16">
         <f>SUM(S7:S11)</f>
-        <v>453.09496347558644</v>
+        <v>544.44444444444457</v>
       </c>
     </row>
     <row r="20" spans="6:13" x14ac:dyDescent="0.3">
@@ -1519,7 +1527,7 @@
       </c>
       <c r="H24">
         <f t="shared" si="10"/>
-        <v>0.4285714285714286</v>
+        <v>1.5</v>
       </c>
       <c r="I24">
         <f t="shared" si="10"/>
@@ -1531,9 +1539,9 @@
       </c>
     </row>
     <row r="25" spans="6:13" x14ac:dyDescent="0.3">
-      <c r="F25">
+      <c r="F25" s="11">
         <f t="shared" ref="F25:J25" si="11">1/F9-1</f>
-        <v>99</v>
+        <v>3</v>
       </c>
       <c r="G25">
         <f t="shared" si="11"/>
@@ -1606,7 +1614,7 @@
   <dimension ref="D6:U27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1707,7 +1715,7 @@
       </c>
       <c r="O7" s="6">
         <f>IF(OR($N$7:$N$11)=0, 2, O8)</f>
-        <v>1.0000000000000009E-2</v>
+        <v>3.999999999999998E-2</v>
       </c>
       <c r="P7" s="6">
         <f>ABS(MIN(F7:J7)-L7)</f>
@@ -1744,7 +1752,7 @@
         <v>0.5</v>
       </c>
       <c r="H8" s="2">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="I8" s="2">
         <v>0.4</v>
@@ -1754,7 +1762,7 @@
       </c>
       <c r="K8" s="3">
         <f t="shared" ref="K8:K11" si="0">SUM(F8:J8)/5</f>
-        <v>0.57999999999999996</v>
+        <v>0.52</v>
       </c>
       <c r="L8" s="4">
         <v>0.35</v>
@@ -1769,7 +1777,7 @@
       </c>
       <c r="O8" s="6">
         <f>ABS($K$7-K8)/2</f>
-        <v>1.0000000000000009E-2</v>
+        <v>3.999999999999998E-2</v>
       </c>
       <c r="P8" s="6">
         <f t="shared" ref="P8:P11" si="2">ABS(MIN(F8:J8)-L8)</f>
@@ -1777,7 +1785,7 @@
       </c>
       <c r="Q8" s="7">
         <f t="shared" ref="Q8:Q11" si="3">(M8*N8/O8)^2</f>
-        <v>9999.9999999999836</v>
+        <v>625.00000000000068</v>
       </c>
       <c r="R8" s="7">
         <f t="shared" ref="R8:R11" si="4">((1-M8)*(1-N8)/P8)^2</f>
@@ -1808,12 +1816,12 @@
       <c r="I9" s="2">
         <v>0.8</v>
       </c>
-      <c r="J9" s="2">
-        <v>0.36</v>
+      <c r="J9" s="10">
+        <v>0.4</v>
       </c>
       <c r="K9" s="3">
         <f t="shared" si="0"/>
-        <v>0.47199999999999998</v>
+        <v>0.48</v>
       </c>
       <c r="L9" s="4">
         <v>0.35</v>
@@ -1828,7 +1836,7 @@
       </c>
       <c r="O9" s="6">
         <f t="shared" ref="O9:O11" si="7">ABS($K$7-K9)/2</f>
-        <v>6.4000000000000001E-2</v>
+        <v>0.06</v>
       </c>
       <c r="P9" s="6">
         <f t="shared" si="2"/>
@@ -1844,7 +1852,7 @@
       </c>
       <c r="S9" s="7">
         <f t="shared" ref="S9:S11" si="8">((1-M9)*N9/MAX(O9, P9))^2</f>
-        <v>244.140625</v>
+        <v>277.77777777777783</v>
       </c>
       <c r="U9" t="b">
         <f t="shared" si="5"/>
@@ -1859,7 +1867,7 @@
         <v>0.34</v>
       </c>
       <c r="G10" s="2">
-        <v>0.34</v>
+        <v>0.9</v>
       </c>
       <c r="H10" s="2">
         <v>0.8</v>
@@ -1872,7 +1880,7 @@
       </c>
       <c r="K10" s="3">
         <f t="shared" si="0"/>
-        <v>0.53599999999999992</v>
+        <v>0.64800000000000002</v>
       </c>
       <c r="L10" s="4">
         <v>0.35</v>
@@ -1883,11 +1891,11 @@
       </c>
       <c r="N10" s="5" t="b">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O10" s="6">
         <f t="shared" si="7"/>
-        <v>3.2000000000000028E-2</v>
+        <v>2.4000000000000021E-2</v>
       </c>
       <c r="P10" s="6">
         <f t="shared" si="2"/>
@@ -1899,11 +1907,11 @@
       </c>
       <c r="R10" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10000.000000000095</v>
       </c>
       <c r="S10" s="7">
         <f t="shared" si="8"/>
-        <v>976.56249999999818</v>
+        <v>0</v>
       </c>
       <c r="U10" t="b">
         <f t="shared" si="5"/>
@@ -1986,19 +1994,19 @@
     <row r="16" spans="4:21" x14ac:dyDescent="0.3">
       <c r="H16">
         <f>1/(MIN($O$7/2,$P$7))^2</f>
-        <v>39999.999999999927</v>
+        <v>2500.0000000000027</v>
       </c>
       <c r="I16">
         <f>SUM(Q7:Q11)</f>
-        <v>9999.9999999999836</v>
+        <v>625.00000000000068</v>
       </c>
       <c r="J16">
         <f>SUM(R7:R11)</f>
-        <v>0</v>
+        <v>10000.000000000095</v>
       </c>
       <c r="K16">
         <f>SUM(S7:S11)</f>
-        <v>5126.9531249999909</v>
+        <v>4184.0277777777701</v>
       </c>
     </row>
     <row r="20" spans="6:13" x14ac:dyDescent="0.3">
@@ -2048,7 +2056,7 @@
       </c>
       <c r="H24">
         <f t="shared" si="10"/>
-        <v>0.4285714285714286</v>
+        <v>1.5</v>
       </c>
       <c r="I24">
         <f t="shared" si="10"/>
@@ -2076,9 +2084,9 @@
         <f t="shared" si="10"/>
         <v>0.25</v>
       </c>
-      <c r="J25">
-        <f t="shared" si="10"/>
-        <v>1.7777777777777777</v>
+      <c r="J25" s="11">
+        <f t="shared" si="10"/>
+        <v>1.5</v>
       </c>
     </row>
     <row r="26" spans="6:13" x14ac:dyDescent="0.3">
@@ -2088,7 +2096,7 @@
       </c>
       <c r="G26">
         <f t="shared" si="10"/>
-        <v>1.9411764705882351</v>
+        <v>0.11111111111111116</v>
       </c>
       <c r="H26">
         <f t="shared" si="10"/>

</xml_diff>